<commit_message>
new method for cal
excel engine use the old xlwt, it may cause problems
</commit_message>
<xml_diff>
--- a/Clus/20220911/test/Clus-DoC Results/ROI_set/after_col_mark/statistics.xlsx
+++ b/Clus/20220911/test/Clus-DoC Results/ROI_set/after_col_mark/statistics.xlsx
@@ -478,54 +478,54 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2148</v>
+        <v>994</v>
       </c>
       <c r="B2" t="n">
-        <v>567</v>
+        <v>331</v>
       </c>
       <c r="C2" t="n">
-        <v>531</v>
+        <v>55</v>
       </c>
       <c r="D2" t="n">
-        <v>1050</v>
+        <v>608</v>
       </c>
       <c r="E2" t="n">
-        <v>717</v>
+        <v>116</v>
       </c>
       <c r="F2" t="n">
-        <v>106</v>
+        <v>24</v>
       </c>
       <c r="G2" t="n">
-        <v>407</v>
+        <v>48</v>
       </c>
       <c r="H2" t="n">
-        <v>204</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3903</v>
+        <v>1319</v>
       </c>
       <c r="B3" t="n">
-        <v>538</v>
+        <v>364</v>
       </c>
       <c r="C3" t="n">
-        <v>1177</v>
+        <v>345</v>
       </c>
       <c r="D3" t="n">
-        <v>2188</v>
+        <v>610</v>
       </c>
       <c r="E3" t="n">
-        <v>1324</v>
+        <v>251</v>
       </c>
       <c r="F3" t="n">
-        <v>134</v>
+        <v>45</v>
       </c>
       <c r="G3" t="n">
-        <v>792</v>
+        <v>139</v>
       </c>
       <c r="H3" t="n">
-        <v>398</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -591,54 +591,54 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>5736</v>
+        <v>1267</v>
       </c>
       <c r="B2" t="n">
-        <v>928</v>
+        <v>322</v>
       </c>
       <c r="C2" t="n">
-        <v>1189</v>
+        <v>234</v>
       </c>
       <c r="D2" t="n">
-        <v>3619</v>
+        <v>711</v>
       </c>
       <c r="E2" t="n">
-        <v>276</v>
+        <v>140</v>
       </c>
       <c r="F2" t="n">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="G2" t="n">
-        <v>180</v>
+        <v>88</v>
       </c>
       <c r="H2" t="n">
-        <v>62</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>9100</v>
+        <v>1655</v>
       </c>
       <c r="B3" t="n">
-        <v>595</v>
+        <v>342</v>
       </c>
       <c r="C3" t="n">
-        <v>1122</v>
+        <v>75</v>
       </c>
       <c r="D3" t="n">
-        <v>7383</v>
+        <v>1238</v>
       </c>
       <c r="E3" t="n">
-        <v>277</v>
+        <v>180</v>
       </c>
       <c r="F3" t="n">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="G3" t="n">
-        <v>131</v>
+        <v>56</v>
       </c>
       <c r="H3" t="n">
-        <v>125</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>